<commit_message>
modify view validated skpi
</commit_message>
<xml_diff>
--- a/public/format_tambah_mahasiswa.xlsx
+++ b/public/format_tambah_mahasiswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SKPI_UNWAHA\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C509E2-FF25-4F18-9052-17738127E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB717061-98B9-4CD7-A84B-0857DC413E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65DF87A5-63C0-4B49-B4E9-32164220339E}"/>
   </bookViews>
@@ -83,9 +83,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,33 +144,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -513,58 +498,57 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
-    <col min="3" max="7" width="21.7109375" style="3" customWidth="1"/>
-    <col min="8" max="10" width="21.7109375" style="4" customWidth="1"/>
-    <col min="11" max="12" width="21.7109375" style="3" customWidth="1"/>
+    <col min="1" max="2" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="7" width="21.7109375" style="2" customWidth="1"/>
+    <col min="8" max="11" width="21.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L2" s="5"/>
+      <c r="L2" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>